<commit_message>
BVA and ECP added for Project 2
</commit_message>
<xml_diff>
--- a/1st project/BVA and ECP.xlsx
+++ b/1st project/BVA and ECP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_portfolio\Maximov_Projects\1st project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0EC0B-4117-4177-BC16-3D42C6B9B82C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40855FF1-63D5-4054-BB07-8ABAD81459E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1339,18 +1339,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1374,15 +1383,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1604,7 +1604,9 @@
   </sheetPr>
   <dimension ref="A1:H1027"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1646,10 +1648,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1670,8 +1672,8 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="113"/>
-      <c r="B3" s="114"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1690,8 +1692,8 @@
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="113"/>
-      <c r="B4" s="117" t="s">
+      <c r="A4" s="116"/>
+      <c r="B4" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1712,8 +1714,8 @@
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
-      <c r="B5" s="113"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="15" t="s">
         <v>20</v>
       </c>
@@ -1732,8 +1734,8 @@
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="113"/>
-      <c r="B6" s="113"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="15" t="s">
         <v>22</v>
       </c>
@@ -1752,8 +1754,8 @@
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113"/>
-      <c r="B7" s="113"/>
+      <c r="A7" s="116"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="15" t="s">
         <v>24</v>
       </c>
@@ -1772,8 +1774,8 @@
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="113"/>
-      <c r="B8" s="113"/>
+      <c r="A8" s="116"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="15" t="s">
         <v>26</v>
       </c>
@@ -1788,8 +1790,8 @@
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
-      <c r="B9" s="113"/>
+      <c r="A9" s="116"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="15" t="s">
         <v>29</v>
       </c>
@@ -1804,8 +1806,8 @@
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113"/>
-      <c r="B10" s="113"/>
+      <c r="A10" s="116"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="23" t="s">
         <v>31</v>
       </c>
@@ -1820,8 +1822,8 @@
       <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="113"/>
-      <c r="B11" s="113"/>
+      <c r="A11" s="116"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="23" t="s">
         <v>32</v>
       </c>
@@ -1836,8 +1838,8 @@
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="113"/>
-      <c r="B12" s="113"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="23" t="s">
         <v>33</v>
       </c>
@@ -1852,8 +1854,8 @@
       <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
-      <c r="B13" s="113"/>
+      <c r="A13" s="116"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="23" t="s">
         <v>35</v>
       </c>
@@ -1868,8 +1870,8 @@
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113"/>
-      <c r="B14" s="114"/>
+      <c r="A14" s="116"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="23" t="s">
         <v>37</v>
       </c>
@@ -1884,8 +1886,8 @@
       <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
-      <c r="B15" s="118" t="s">
+      <c r="A15" s="116"/>
+      <c r="B15" s="121" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -1902,8 +1904,8 @@
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
-      <c r="B16" s="119"/>
+      <c r="A16" s="117"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="26" t="s">
         <v>41</v>
       </c>
@@ -1928,10 +1930,10 @@
       <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="112" t="s">
+      <c r="A18" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1952,8 +1954,8 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="114"/>
+      <c r="A19" s="116"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
@@ -1972,8 +1974,8 @@
       <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="113"/>
-      <c r="B20" s="117" t="s">
+      <c r="A20" s="116"/>
+      <c r="B20" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -1994,8 +1996,8 @@
       <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="113"/>
-      <c r="B21" s="113"/>
+      <c r="A21" s="116"/>
+      <c r="B21" s="116"/>
       <c r="C21" s="15" t="s">
         <v>20</v>
       </c>
@@ -2014,8 +2016,8 @@
       <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="113"/>
-      <c r="B22" s="113"/>
+      <c r="A22" s="116"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="15" t="s">
         <v>46</v>
       </c>
@@ -2034,8 +2036,8 @@
       <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="113"/>
-      <c r="B23" s="113"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="15" t="s">
         <v>24</v>
       </c>
@@ -2054,8 +2056,8 @@
       <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="113"/>
-      <c r="B24" s="113"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="15" t="s">
         <v>26</v>
       </c>
@@ -2070,8 +2072,8 @@
       <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="113"/>
-      <c r="B25" s="113"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="116"/>
       <c r="C25" s="15" t="s">
         <v>29</v>
       </c>
@@ -2086,8 +2088,8 @@
       <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113"/>
-      <c r="B26" s="113"/>
+      <c r="A26" s="116"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="23" t="s">
         <v>31</v>
       </c>
@@ -2102,8 +2104,8 @@
       <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113"/>
-      <c r="B27" s="113"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="116"/>
       <c r="C27" s="23" t="s">
         <v>32</v>
       </c>
@@ -2118,8 +2120,8 @@
       <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="113"/>
-      <c r="B28" s="113"/>
+      <c r="A28" s="116"/>
+      <c r="B28" s="116"/>
       <c r="C28" s="23" t="s">
         <v>33</v>
       </c>
@@ -2134,8 +2136,8 @@
       <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="113"/>
-      <c r="B29" s="113"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="116"/>
       <c r="C29" s="23" t="s">
         <v>35</v>
       </c>
@@ -2150,8 +2152,8 @@
       <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="113"/>
-      <c r="B30" s="114"/>
+      <c r="A30" s="116"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="23" t="s">
         <v>37</v>
       </c>
@@ -2166,8 +2168,8 @@
       <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="113"/>
-      <c r="B31" s="117" t="s">
+      <c r="A31" s="116"/>
+      <c r="B31" s="119" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -2184,8 +2186,8 @@
       <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="114"/>
-      <c r="B32" s="114"/>
+      <c r="A32" s="117"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="7" t="s">
         <v>41</v>
       </c>
@@ -2213,7 +2215,7 @@
       <c r="A34" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="45" t="s">
@@ -2234,8 +2236,8 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="114"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="117"/>
       <c r="C35" s="49" t="s">
         <v>54</v>
       </c>
@@ -2254,8 +2256,8 @@
       <c r="H35" s="52"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="113"/>
-      <c r="B36" s="117" t="s">
+      <c r="A36" s="116"/>
+      <c r="B36" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="53" t="s">
@@ -2272,8 +2274,8 @@
       <c r="H36" s="35"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="113"/>
-      <c r="B37" s="113"/>
+      <c r="A37" s="116"/>
+      <c r="B37" s="116"/>
       <c r="C37" s="54" t="s">
         <v>59</v>
       </c>
@@ -2288,8 +2290,8 @@
       <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="113"/>
-      <c r="B38" s="113"/>
+      <c r="A38" s="116"/>
+      <c r="B38" s="116"/>
       <c r="C38" s="54" t="s">
         <v>61</v>
       </c>
@@ -2304,8 +2306,8 @@
       <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="113"/>
-      <c r="B39" s="113"/>
+      <c r="A39" s="116"/>
+      <c r="B39" s="116"/>
       <c r="C39" s="54" t="s">
         <v>63</v>
       </c>
@@ -2320,8 +2322,8 @@
       <c r="H39" s="37"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="113"/>
-      <c r="B40" s="113"/>
+      <c r="A40" s="116"/>
+      <c r="B40" s="116"/>
       <c r="C40" s="54" t="s">
         <v>65</v>
       </c>
@@ -2336,8 +2338,8 @@
       <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="113"/>
-      <c r="B41" s="113"/>
+      <c r="A41" s="116"/>
+      <c r="B41" s="116"/>
       <c r="C41" s="54" t="s">
         <v>67</v>
       </c>
@@ -2352,8 +2354,8 @@
       <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="113"/>
-      <c r="B42" s="113"/>
+      <c r="A42" s="116"/>
+      <c r="B42" s="116"/>
       <c r="C42" s="54" t="s">
         <v>69</v>
       </c>
@@ -2368,8 +2370,8 @@
       <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="113"/>
-      <c r="B43" s="113"/>
+      <c r="A43" s="116"/>
+      <c r="B43" s="116"/>
       <c r="C43" s="54" t="s">
         <v>71</v>
       </c>
@@ -2384,8 +2386,8 @@
       <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="113"/>
-      <c r="B44" s="113"/>
+      <c r="A44" s="116"/>
+      <c r="B44" s="116"/>
       <c r="C44" s="57" t="s">
         <v>73</v>
       </c>
@@ -2400,8 +2402,8 @@
       <c r="H44" s="60"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="113"/>
-      <c r="B45" s="113"/>
+      <c r="A45" s="116"/>
+      <c r="B45" s="116"/>
       <c r="C45" s="61" t="s">
         <v>37</v>
       </c>
@@ -2416,8 +2418,8 @@
       <c r="H45" s="52"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="113"/>
-      <c r="B46" s="114"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="117"/>
       <c r="C46" s="62" t="s">
         <v>76</v>
       </c>
@@ -2432,8 +2434,8 @@
       <c r="H46" s="65"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="113"/>
-      <c r="B47" s="117" t="s">
+      <c r="A47" s="116"/>
+      <c r="B47" s="119" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="66" t="s">
@@ -2450,8 +2452,8 @@
       <c r="H47" s="35"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="114"/>
-      <c r="B48" s="114"/>
+      <c r="A48" s="117"/>
+      <c r="B48" s="117"/>
       <c r="C48" s="68" t="s">
         <v>41</v>
       </c>
@@ -2479,7 +2481,7 @@
       <c r="A50" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="45" t="s">
@@ -2500,8 +2502,8 @@
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="113"/>
-      <c r="B51" s="114"/>
+      <c r="A51" s="116"/>
+      <c r="B51" s="117"/>
       <c r="C51" s="49" t="s">
         <v>54</v>
       </c>
@@ -2520,8 +2522,8 @@
       <c r="H51" s="52"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="113"/>
-      <c r="B52" s="117" t="s">
+      <c r="A52" s="116"/>
+      <c r="B52" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="53" t="s">
@@ -2538,8 +2540,8 @@
       <c r="H52" s="35"/>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
-      <c r="B53" s="113"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="116"/>
       <c r="C53" s="54" t="s">
         <v>59</v>
       </c>
@@ -2554,8 +2556,8 @@
       <c r="H53" s="37"/>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="113"/>
-      <c r="B54" s="113"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="116"/>
       <c r="C54" s="54" t="s">
         <v>61</v>
       </c>
@@ -2570,8 +2572,8 @@
       <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="113"/>
-      <c r="B55" s="113"/>
+      <c r="A55" s="116"/>
+      <c r="B55" s="116"/>
       <c r="C55" s="54" t="s">
         <v>63</v>
       </c>
@@ -2586,8 +2588,8 @@
       <c r="H55" s="37"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="113"/>
-      <c r="B56" s="113"/>
+      <c r="A56" s="116"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="54" t="s">
         <v>65</v>
       </c>
@@ -2602,8 +2604,8 @@
       <c r="H56" s="37"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="113"/>
-      <c r="B57" s="113"/>
+      <c r="A57" s="116"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="54" t="s">
         <v>67</v>
       </c>
@@ -2618,8 +2620,8 @@
       <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
-      <c r="B58" s="113"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="54" t="s">
         <v>69</v>
       </c>
@@ -2634,8 +2636,8 @@
       <c r="H58" s="37"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="113"/>
-      <c r="B59" s="113"/>
+      <c r="A59" s="116"/>
+      <c r="B59" s="116"/>
       <c r="C59" s="54" t="s">
         <v>71</v>
       </c>
@@ -2650,8 +2652,8 @@
       <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="113"/>
-      <c r="B60" s="113"/>
+      <c r="A60" s="116"/>
+      <c r="B60" s="116"/>
       <c r="C60" s="57" t="s">
         <v>73</v>
       </c>
@@ -2666,8 +2668,8 @@
       <c r="H60" s="60"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="113"/>
-      <c r="B61" s="113"/>
+      <c r="A61" s="116"/>
+      <c r="B61" s="116"/>
       <c r="C61" s="61" t="s">
         <v>37</v>
       </c>
@@ -2682,8 +2684,8 @@
       <c r="H61" s="52"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="113"/>
-      <c r="B62" s="114"/>
+      <c r="A62" s="116"/>
+      <c r="B62" s="117"/>
       <c r="C62" s="62" t="s">
         <v>76</v>
       </c>
@@ -2698,8 +2700,8 @@
       <c r="H62" s="65"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="113"/>
-      <c r="B63" s="117" t="s">
+      <c r="A63" s="116"/>
+      <c r="B63" s="119" t="s">
         <v>39</v>
       </c>
       <c r="C63" s="66" t="s">
@@ -2716,8 +2718,8 @@
       <c r="H63" s="35"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="114"/>
-      <c r="B64" s="114"/>
+      <c r="A64" s="117"/>
+      <c r="B64" s="117"/>
       <c r="C64" s="68" t="s">
         <v>41</v>
       </c>
@@ -12369,6 +12371,8 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A18:A32"/>
+    <mergeCell ref="B20:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A34:A48"/>
     <mergeCell ref="A50:A64"/>
     <mergeCell ref="B34:B35"/>
@@ -12377,8 +12381,6 @@
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B62"/>
     <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B20:B30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -12392,7 +12394,7 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -12409,11 +12411,11 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="74"/>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="123" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="121"/>
-      <c r="D1" s="122"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="125"/>
       <c r="E1" s="75"/>
     </row>
     <row r="2" spans="1:28" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -12424,20 +12426,20 @@
       <c r="C2" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="123" t="s">
+      <c r="D2" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="124"/>
+      <c r="E2" s="127"/>
     </row>
     <row r="3" spans="1:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="76"/>
       <c r="B3" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="128" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="124"/>
+      <c r="D3" s="127"/>
       <c r="E3" s="80" t="s">
         <v>87</v>
       </c>
@@ -12449,7 +12451,7 @@
       <c r="D4" s="81"/>
       <c r="E4" s="75"/>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -12473,7 +12475,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="129" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="82" t="s">
@@ -12490,7 +12492,7 @@
       <c r="G6" s="87"/>
     </row>
     <row r="7" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
+      <c r="A7" s="130"/>
       <c r="B7" s="88" t="s">
         <v>92</v>
       </c>
@@ -12526,7 +12528,7 @@
       <c r="AB7" s="92"/>
     </row>
     <row r="8" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="93" t="s">
         <v>94</v>
       </c>
@@ -12562,7 +12564,7 @@
       <c r="AB8" s="92"/>
     </row>
     <row r="9" spans="1:28" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="132" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="97" t="s">
@@ -12577,7 +12579,7 @@
       <c r="E9" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="130" t="s">
+      <c r="F9" s="112" t="s">
         <v>99</v>
       </c>
       <c r="G9" s="101" t="s">
@@ -12585,7 +12587,7 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="127"/>
+      <c r="A10" s="130"/>
       <c r="B10" s="102" t="s">
         <v>101</v>
       </c>
@@ -12598,7 +12600,7 @@
       <c r="E10" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="131" t="s">
+      <c r="F10" s="113" t="s">
         <v>103</v>
       </c>
       <c r="G10" s="106" t="s">
@@ -12606,7 +12608,7 @@
       </c>
     </row>
     <row r="11" spans="1:28" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127"/>
+      <c r="A11" s="130"/>
       <c r="B11" s="102" t="s">
         <v>105</v>
       </c>
@@ -12619,7 +12621,7 @@
       <c r="E11" s="105" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="131" t="s">
+      <c r="F11" s="113" t="s">
         <v>107</v>
       </c>
       <c r="G11" s="106" t="s">
@@ -12627,7 +12629,7 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="127"/>
+      <c r="A12" s="130"/>
       <c r="B12" s="102" t="s">
         <v>109</v>
       </c>
@@ -12640,7 +12642,7 @@
       <c r="E12" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="131" t="s">
+      <c r="F12" s="113" t="s">
         <v>111</v>
       </c>
       <c r="G12" s="106" t="s">
@@ -12648,7 +12650,7 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="107" t="s">
         <v>113</v>
       </c>
@@ -12661,7 +12663,7 @@
       <c r="E13" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="F13" s="132" t="s">
+      <c r="F13" s="114" t="s">
         <v>116</v>
       </c>
       <c r="G13" s="111" t="s">

</xml_diff>